<commit_message>
增加monsterskill_Library 技能 csv json
</commit_message>
<xml_diff>
--- a/design_Doc/Parameter table/condition_Library 状态表.xlsx
+++ b/design_Doc/Parameter table/condition_Library 状态表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C56AEFF-C0DA-4D4F-B15B-6B00E83D37AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312ED091-AE3F-4C06-A018-8DA23BA16569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -683,6 +683,9 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="I3" t="s">
         <v>32</v>
       </c>
@@ -715,6 +718,9 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
       <c r="I4" t="s">
         <v>33</v>
       </c>
@@ -782,6 +788,9 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
@@ -812,6 +821,9 @@
         <v>1</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">

</xml_diff>